<commit_message>
Delete calculoTasaContagio(). Add calculoMortalidad(). Change Salud statechart.
</commit_message>
<xml_diff>
--- a/Data/Provincias.xlsx
+++ b/Data/Provincias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patricio.ivan.pipp\Desktop\COVID Contagion Argentina\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646A9548-F829-4A86-AC4F-8167E6A9B85B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C24010A-1775-4B41-BA08-DB964187E5A7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
@@ -661,7 +661,7 @@
         <v>2.5</v>
       </c>
       <c r="I4">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -691,7 +691,7 @@
         <v>2.5</v>
       </c>
       <c r="I5">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -721,7 +721,7 @@
         <v>2.5</v>
       </c>
       <c r="I6">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -751,7 +751,7 @@
         <v>2.5</v>
       </c>
       <c r="I7">
-        <v>1000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -781,7 +781,7 @@
         <v>2.5</v>
       </c>
       <c r="I8">
-        <v>1000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -811,7 +811,7 @@
         <v>2.5</v>
       </c>
       <c r="I9">
-        <v>1000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -841,7 +841,7 @@
         <v>2.5</v>
       </c>
       <c r="I10">
-        <v>1000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -871,7 +871,7 @@
         <v>2.5</v>
       </c>
       <c r="I11">
-        <v>1000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -901,7 +901,7 @@
         <v>2.5</v>
       </c>
       <c r="I12">
-        <v>1000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -931,7 +931,7 @@
         <v>2.5</v>
       </c>
       <c r="I13">
-        <v>1000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -961,7 +961,7 @@
         <v>2.5</v>
       </c>
       <c r="I14">
-        <v>1000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -991,7 +991,7 @@
         <v>2.5</v>
       </c>
       <c r="I15">
-        <v>1000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1021,7 +1021,7 @@
         <v>2.5</v>
       </c>
       <c r="I16">
-        <v>1000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1051,7 +1051,7 @@
         <v>2.5</v>
       </c>
       <c r="I17">
-        <v>1000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1081,7 +1081,7 @@
         <v>2.5</v>
       </c>
       <c r="I18">
-        <v>1000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1111,7 +1111,7 @@
         <v>2.5</v>
       </c>
       <c r="I19">
-        <v>1000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1141,7 +1141,7 @@
         <v>2.5</v>
       </c>
       <c r="I20">
-        <v>1000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1171,7 +1171,7 @@
         <v>2.5</v>
       </c>
       <c r="I21">
-        <v>1000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1201,7 +1201,7 @@
         <v>2.5</v>
       </c>
       <c r="I22">
-        <v>1000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1231,7 +1231,7 @@
         <v>2.5</v>
       </c>
       <c r="I23">
-        <v>1000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1261,7 +1261,7 @@
         <v>2.5</v>
       </c>
       <c r="I24">
-        <v>1000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1291,7 +1291,7 @@
         <v>2.5</v>
       </c>
       <c r="I25">
-        <v>1000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1321,7 +1321,7 @@
         <v>2.5</v>
       </c>
       <c r="I26">
-        <v>1000</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Read excel file with input data
</commit_message>
<xml_diff>
--- a/Data/Provincias.xlsx
+++ b/Data/Provincias.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patricio.ivan.pipp\Desktop\COVID Contagion Argentina\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C24010A-1775-4B41-BA08-DB964187E5A7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454A39A9-C433-4872-8E4D-D606FF495468}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
   <sheets>
     <sheet name="Provincias" sheetId="1" r:id="rId1"/>
-    <sheet name="Perfil Etário" sheetId="2" r:id="rId2"/>
-    <sheet name="matrizOD" sheetId="3" r:id="rId3"/>
+    <sheet name="Enfermedad" sheetId="4" r:id="rId2"/>
+    <sheet name="tasaMortalidad" sheetId="5" r:id="rId3"/>
+    <sheet name="Perfil Etário" sheetId="2" r:id="rId4"/>
+    <sheet name="matrizOD" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Perfil Etário'!$A$1:$F$2725</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Perfil Etário'!$A$1:$F$2725</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="87">
   <si>
     <t>id</t>
   </si>
@@ -157,12 +159,156 @@
   <si>
     <t>Disponibilidad respiradores</t>
   </si>
+  <si>
+    <t>Concepto</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Comentarios data</t>
+  </si>
+  <si>
+    <t>Fuente</t>
+  </si>
+  <si>
+    <t>tasa_diag_sintom_sobre_diag_total</t>
+  </si>
+  <si>
+    <t>Tasa diagnosticados sintomáticos sobre diagnosticados totales</t>
+  </si>
+  <si>
+    <t>Imperial College COVID-19 paper.</t>
+  </si>
+  <si>
+    <t>tasa_contagio_asinto_sobre_sinto</t>
+  </si>
+  <si>
+    <t>Tasa de contagio entre pacientes asintomátiicos sobre pacientes sintomáticos</t>
+  </si>
+  <si>
+    <t>tasa_diag_sobre_infectados</t>
+  </si>
+  <si>
+    <t>Tasa diagnosticados sobre infectados totales</t>
+  </si>
+  <si>
+    <t>40-50%</t>
+  </si>
+  <si>
+    <t>tasa_criticos_sobre_diag</t>
+  </si>
+  <si>
+    <t>Tasa casos críticos sobre diagnosticados totales</t>
+  </si>
+  <si>
+    <t>https://www.who.int/news-room/detail/23-01-2020-statement-on-the-meeting-of-the-international-health-regulations-(2005)-emergency-committee-regarding-the-outbreak-of-novel-coronavirus-(2019-ncov)</t>
+  </si>
+  <si>
+    <t>tasa_hospitalizacion</t>
+  </si>
+  <si>
+    <t>Tasa hospitalización</t>
+  </si>
+  <si>
+    <t>Ver tabla por rango etario. Imperial College COVID-19 paper.</t>
+  </si>
+  <si>
+    <t>tasa_terapia</t>
+  </si>
+  <si>
+    <t>Tasa terapia intensiva</t>
+  </si>
+  <si>
+    <t>tasa_respirador</t>
+  </si>
+  <si>
+    <t>Tasa respirador</t>
+  </si>
+  <si>
+    <t>tasa_mortandad</t>
+  </si>
+  <si>
+    <t>Tasa mortandad</t>
+  </si>
+  <si>
+    <t>ver datos rango etario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.worldometers.info/coronavirus/coronavirus-death-rate/  </t>
+  </si>
+  <si>
+    <t>dur_incubacion</t>
+  </si>
+  <si>
+    <t>Duracion incubacion</t>
+  </si>
+  <si>
+    <t>5,1 dias</t>
+  </si>
+  <si>
+    <t>dur_casos_mortales</t>
+  </si>
+  <si>
+    <t>Duración enfermedad para casos mortales</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>14-56 dias</t>
+  </si>
+  <si>
+    <t>https://www.who.int/docs/default-source/coronaviruse/who-china-joint-mission-on-covid-19-final-report.pdf</t>
+  </si>
+  <si>
+    <t>dur_casos_leves</t>
+  </si>
+  <si>
+    <t>Duración efermedad para casos leves</t>
+  </si>
+  <si>
+    <t>14 dias</t>
+  </si>
+  <si>
+    <t>dur_casos_graves</t>
+  </si>
+  <si>
+    <t>Duración enfermedad para casos graves</t>
+  </si>
+  <si>
+    <t>21- 42 dias</t>
+  </si>
+  <si>
+    <t>dur_hosp_pac_grave</t>
+  </si>
+  <si>
+    <t>Tiempo medio de hospitalización para un paciente grave</t>
+  </si>
+  <si>
+    <t>16 dias</t>
+  </si>
+  <si>
+    <t>dur_hosp_pac_leve</t>
+  </si>
+  <si>
+    <t>Tiempo medio de hospitalización para un paciente leve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 dias </t>
+  </si>
+  <si>
+    <t>Probabilidad de muerte</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,16 +333,44 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -204,24 +378,75 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{020520A6-6A09-4919-9919-36C8A652F88B}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{D0623323-BFFB-44CA-A557-18A3E101DA7F}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{D1AD94BC-AD13-4C7B-9337-AC3187EAAF7F}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -535,7 +760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBFD61EF-8890-4F24-B0B0-4C71ECA915F1}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1331,6 +1556,368 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46DDACF-D0ED-4CB1-BA1F-87BB8EEFE26F}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="198.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
+      <c r="A2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75">
+      <c r="A3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75">
+      <c r="A4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.45</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75">
+      <c r="A5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75">
+      <c r="A6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="7">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75">
+      <c r="A7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75">
+      <c r="A8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75">
+      <c r="A9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="7">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75">
+      <c r="A10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75">
+      <c r="A11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75">
+      <c r="A12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="7">
+        <v>14</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75">
+      <c r="A13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75">
+      <c r="A14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="6">
+        <v>16</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75">
+      <c r="A15" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="6">
+        <v>8</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD688DC-0BC2-43C0-9843-BCA0B9570887}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="11">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="11">
+        <v>10</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="11">
+        <v>20</v>
+      </c>
+      <c r="B4" s="12">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="11">
+        <v>30</v>
+      </c>
+      <c r="B5" s="12">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="11">
+        <v>40</v>
+      </c>
+      <c r="B6" s="12">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="11">
+        <v>50</v>
+      </c>
+      <c r="B7" s="12">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="11">
+        <v>60</v>
+      </c>
+      <c r="B8" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="11">
+        <v>70</v>
+      </c>
+      <c r="B9" s="12">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="11">
+        <v>80</v>
+      </c>
+      <c r="B10" s="12">
+        <v>9.2999999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8EFC4FE-610E-497E-93FF-F825D6C88A88}">
   <dimension ref="A1:F2725"/>
   <sheetViews>
@@ -61300,7 +61887,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2624E291-BFC7-4313-ACE8-D415BC869A1A}">
   <dimension ref="A1:Z26"/>
   <sheetViews>

</xml_diff>

<commit_message>
adds gradeAtencionActual & Requerido, minor changes
</commit_message>
<xml_diff>
--- a/Data/Provincias.xlsx
+++ b/Data/Provincias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCDD26E-37C7-4212-BB75-553B7EC7275A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1626289-FE77-4667-9AFC-CDFD018A35EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
   <sheets>
     <sheet name="Provincias" sheetId="1" r:id="rId1"/>
@@ -558,12 +558,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -581,6 +575,12 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -902,12 +902,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBFD61EF-8890-4F24-B0B0-4C71ECA915F1}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1701,7 +1704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46DDACF-D0ED-4CB1-BA1F-87BB8EEFE26F}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -1712,7 +1715,7 @@
     <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="198.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="33"/>
+    <col min="6" max="8" width="8.88671875" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18">
@@ -1745,15 +1748,15 @@
       <c r="C2" s="14">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" ht="15.6">
       <c r="A3" s="17" t="s">
@@ -1769,9 +1772,9 @@
       <c r="E3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="15.6">
       <c r="A4" s="22" t="s">
@@ -1789,9 +1792,9 @@
       <c r="E4" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
     </row>
     <row r="5" spans="1:8" ht="15.6">
       <c r="A5" s="17" t="s">
@@ -1807,9 +1810,9 @@
       <c r="E5" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" spans="1:8" ht="15.6">
       <c r="A6" s="9" t="s">
@@ -1827,9 +1830,9 @@
       <c r="E6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" ht="15.6">
       <c r="A7" s="9" t="s">
@@ -1847,9 +1850,9 @@
       <c r="E7" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="1:8" ht="46.8">
       <c r="A8" s="9" t="s">
@@ -1867,9 +1870,9 @@
       <c r="E8" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:8" ht="15.6">
       <c r="A9" s="9" t="s">
@@ -1884,12 +1887,12 @@
       <c r="D9" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="15.6">
       <c r="A10" s="9" t="s">
@@ -1907,9 +1910,9 @@
       <c r="E10" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" ht="15.6">
       <c r="A11" s="12" t="s">
@@ -1927,9 +1930,9 @@
       <c r="E11" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="12" spans="1:8" ht="15.6">
       <c r="A12" s="9" t="s">
@@ -1947,9 +1950,9 @@
       <c r="E12" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" ht="15.6">
       <c r="A13" s="9" t="s">
@@ -1961,15 +1964,15 @@
       <c r="C13" s="16">
         <v>21</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="33">
         <v>42</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
     </row>
     <row r="14" spans="1:8" ht="15.6">
       <c r="A14" s="17" t="s">
@@ -1981,15 +1984,15 @@
       <c r="C14" s="19">
         <v>16</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="34" t="s">
         <v>89</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" spans="1:8" ht="15.6">
       <c r="A15" s="17" t="s">
@@ -2001,13 +2004,13 @@
       <c r="C15" s="19">
         <v>8</v>
       </c>
-      <c r="D15" s="26"/>
+      <c r="D15" s="35"/>
       <c r="E15" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Read hospital beds and other information from Excel file
</commit_message>
<xml_diff>
--- a/Data/Provincias.xlsx
+++ b/Data/Provincias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patricio.ivan.pipp\Desktop\COVID Contagion Argentina\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D2D629-40FE-4DD9-B1AB-A7A98F604205}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FF804C-B90F-42AF-AB88-292C04CF95FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="94">
   <si>
     <t>id</t>
   </si>
@@ -316,6 +316,12 @@
   </si>
   <si>
     <t>Infectados confirmados iniciales</t>
+  </si>
+  <si>
+    <t>Camas Aislamiento</t>
+  </si>
+  <si>
+    <t>Cama terapia intensiva</t>
   </si>
 </sst>
 </file>
@@ -903,19 +909,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBFD61EF-8890-4F24-B0B0-4C71ECA915F1}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -946,8 +957,15 @@
       <c r="J1" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1</v>
       </c>
@@ -978,10 +996,17 @@
         <v>1000</v>
       </c>
       <c r="J2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>100</v>
+      </c>
+      <c r="K2">
+        <v>50</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1012,10 +1037,17 @@
         <v>1000</v>
       </c>
       <c r="J3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>100</v>
+      </c>
+      <c r="K3">
+        <v>50</v>
+      </c>
+      <c r="L3">
+        <v>50</v>
+      </c>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1047,8 +1079,14 @@
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4">
+        <v>50</v>
+      </c>
+      <c r="L4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1080,8 +1118,14 @@
       <c r="J5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5">
+        <v>50</v>
+      </c>
+      <c r="L5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1111,10 +1155,16 @@
         <v>500</v>
       </c>
       <c r="J6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>100</v>
+      </c>
+      <c r="K6">
+        <v>50</v>
+      </c>
+      <c r="L6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1146,8 +1196,14 @@
       <c r="J7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7">
+        <v>50</v>
+      </c>
+      <c r="L7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1179,8 +1235,14 @@
       <c r="J8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8">
+        <v>50</v>
+      </c>
+      <c r="L8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1212,8 +1274,14 @@
       <c r="J9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9">
+        <v>50</v>
+      </c>
+      <c r="L9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1245,8 +1313,14 @@
       <c r="J10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10">
+        <v>50</v>
+      </c>
+      <c r="L10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1278,8 +1352,14 @@
       <c r="J11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11">
+        <v>50</v>
+      </c>
+      <c r="L11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1311,8 +1391,14 @@
       <c r="J12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12">
+        <v>50</v>
+      </c>
+      <c r="L12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1344,8 +1430,14 @@
       <c r="J13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13">
+        <v>50</v>
+      </c>
+      <c r="L13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1377,8 +1469,14 @@
       <c r="J14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14">
+        <v>50</v>
+      </c>
+      <c r="L14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1410,8 +1508,14 @@
       <c r="J15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15">
+        <v>50</v>
+      </c>
+      <c r="L15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1443,8 +1547,14 @@
       <c r="J16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16">
+        <v>50</v>
+      </c>
+      <c r="L16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1476,8 +1586,14 @@
       <c r="J17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17">
+        <v>50</v>
+      </c>
+      <c r="L17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1509,8 +1625,14 @@
       <c r="J18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18">
+        <v>50</v>
+      </c>
+      <c r="L18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1542,8 +1664,14 @@
       <c r="J19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19">
+        <v>50</v>
+      </c>
+      <c r="L19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1575,8 +1703,14 @@
       <c r="J20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20">
+        <v>50</v>
+      </c>
+      <c r="L20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1608,8 +1742,14 @@
       <c r="J21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21">
+        <v>50</v>
+      </c>
+      <c r="L21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1641,8 +1781,14 @@
       <c r="J22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22">
+        <v>50</v>
+      </c>
+      <c r="L22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1674,8 +1820,14 @@
       <c r="J23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23">
+        <v>50</v>
+      </c>
+      <c r="L23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1707,8 +1859,14 @@
       <c r="J24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24">
+        <v>50</v>
+      </c>
+      <c r="L24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1740,8 +1898,14 @@
       <c r="J25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25">
+        <v>50</v>
+      </c>
+      <c r="L25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1772,6 +1936,12 @@
       </c>
       <c r="J26">
         <v>0</v>
+      </c>
+      <c r="K26">
+        <v>50</v>
+      </c>
+      <c r="L26">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add calculoAgravamiento(). Change calculoMortalidad().
</commit_message>
<xml_diff>
--- a/Data/Provincias.xlsx
+++ b/Data/Provincias.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patricio.ivan.pipp\Desktop\COVID Contagion Argentina\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FF804C-B90F-42AF-AB88-292C04CF95FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C64830-A77A-4E8E-A93D-D726FCA5CBE4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="4" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
   <sheets>
     <sheet name="Provincias" sheetId="1" r:id="rId1"/>
     <sheet name="Enfermedad" sheetId="4" r:id="rId2"/>
-    <sheet name="tasaMortalidad" sheetId="5" r:id="rId3"/>
-    <sheet name="tasaHospitalizacion" sheetId="6" r:id="rId4"/>
-    <sheet name="tasaTerapiaIntensiva" sheetId="7" r:id="rId5"/>
-    <sheet name="Perfil Etário" sheetId="2" r:id="rId6"/>
-    <sheet name="matrizOD" sheetId="3" r:id="rId7"/>
+    <sheet name="tasaMortalidadLeve" sheetId="5" r:id="rId3"/>
+    <sheet name="tasaMortalidadGrave" sheetId="8" r:id="rId4"/>
+    <sheet name="agravamiento" sheetId="9" r:id="rId5"/>
+    <sheet name="tasaHospitalizacion" sheetId="6" r:id="rId6"/>
+    <sheet name="tasaTerapiaIntensiva" sheetId="7" r:id="rId7"/>
+    <sheet name="Perfil Etário" sheetId="2" r:id="rId8"/>
+    <sheet name="matrizOD" sheetId="3" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Perfil Etário'!$A$1:$F$2725</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Perfil Etário'!$A$1:$F$2725</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="97">
   <si>
     <t>id</t>
   </si>
@@ -322,6 +324,15 @@
   </si>
   <si>
     <t>Cama terapia intensiva</t>
+  </si>
+  <si>
+    <t>asistencia_necesaria</t>
+  </si>
+  <si>
+    <t>asistencia_recibida</t>
+  </si>
+  <si>
+    <t>probabilidad de morir recibiendo respectivo tattamientto</t>
   </si>
 </sst>
 </file>
@@ -911,7 +922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBFD61EF-8890-4F24-B0B0-4C71ECA915F1}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2279,9 +2290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD688DC-0BC2-43C0-9843-BCA0B9570887}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2376,6 +2385,244 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5C39B9-311D-46EB-8C4B-C17C1C794B92}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="6">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="6">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="6">
+        <v>20</v>
+      </c>
+      <c r="B4" s="7">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="6">
+        <v>30</v>
+      </c>
+      <c r="B5" s="7">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="6">
+        <v>40</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="6">
+        <v>50</v>
+      </c>
+      <c r="B7" s="7">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="6">
+        <v>60</v>
+      </c>
+      <c r="B8" s="7">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="6">
+        <v>70</v>
+      </c>
+      <c r="B9" s="7">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="6">
+        <v>80</v>
+      </c>
+      <c r="B10" s="7">
+        <v>9.2999999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A334587-EE99-4B44-B70D-1A4CADF34D80}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="6">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="6">
+        <v>3</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="6">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="6">
+        <v>3</v>
+      </c>
+      <c r="B11" s="6">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B4B6E2-9FA7-455F-8FBF-E034CDFC18C4}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -2475,7 +2722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB52A6C-EEE2-4A48-ACFA-1E58998BAFDB}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -2574,7 +2821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8EFC4FE-610E-497E-93FF-F825D6C88A88}">
   <dimension ref="A1:F2725"/>
   <sheetViews>
@@ -62544,7 +62791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2624E291-BFC7-4313-ACE8-D415BC869A1A}">
   <dimension ref="A1:Z26"/>
   <sheetViews>

</xml_diff>

<commit_message>
Cambios en creacion de agentes iniciales y vuelta para atras en contagios
</commit_message>
<xml_diff>
--- a/Data/Provincias.xlsx
+++ b/Data/Provincias.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patricio.ivan.pipp\Desktop\COVID Contagion Argentina\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9933FDD-8542-4CB1-93B6-EABC487A9FE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623D8E2C-7760-42D6-B9B1-A14FAD9D70A0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="9" activeTab="10" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
   <sheets>
     <sheet name="Provincias" sheetId="1" r:id="rId1"/>
@@ -1044,12 +1044,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1072,17 +1066,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -1407,21 +1407,19 @@
   </sheetPr>
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1549,7 +1547,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="46" t="s">
         <v>129</v>
       </c>
       <c r="C4">
@@ -1627,7 +1625,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="46" t="s">
         <v>7</v>
       </c>
       <c r="C6">
@@ -1705,7 +1703,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="46" t="s">
         <v>9</v>
       </c>
       <c r="C8">
@@ -1744,7 +1742,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="46" t="s">
         <v>212</v>
       </c>
       <c r="C9">
@@ -2056,7 +2054,7 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="46" t="s">
         <v>18</v>
       </c>
       <c r="C17">
@@ -2095,7 +2093,7 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="46" t="s">
         <v>19</v>
       </c>
       <c r="C18">
@@ -2459,120 +2457,120 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="36">
+      <c r="A2" s="34">
         <v>0</v>
       </c>
-      <c r="B2" s="37">
+      <c r="B2" s="35">
         <v>0</v>
       </c>
-      <c r="C2" s="38">
+      <c r="C2" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="36">
+      <c r="A3" s="34">
         <v>10</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="35">
         <v>1E-4</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="36">
         <v>2E-3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="36">
+      <c r="A4" s="34">
         <v>20</v>
       </c>
-      <c r="B4" s="37">
+      <c r="B4" s="35">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="36">
         <v>2E-3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="36">
+      <c r="A5" s="34">
         <v>30</v>
       </c>
-      <c r="B5" s="37">
+      <c r="B5" s="35">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="36">
         <v>2E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="36">
+      <c r="A6" s="34">
         <v>40</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B6" s="35">
         <v>1.5E-3</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="36">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="36">
+      <c r="A7" s="34">
         <v>50</v>
       </c>
-      <c r="B7" s="37">
+      <c r="B7" s="35">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="36">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="36">
+      <c r="A8" s="34">
         <v>60</v>
       </c>
-      <c r="B8" s="37">
+      <c r="B8" s="35">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="36">
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="36">
+      <c r="A9" s="34">
         <v>70</v>
       </c>
-      <c r="B9" s="37">
+      <c r="B9" s="35">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="36">
         <v>0.08</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="36">
+      <c r="A10" s="34">
         <v>80</v>
       </c>
-      <c r="B10" s="37">
+      <c r="B10" s="35">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="36">
         <v>0.14799999999999999</v>
       </c>
     </row>
@@ -2589,15 +2587,15 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2618,7 +2616,7 @@
       <c r="B2" s="6">
         <v>0</v>
       </c>
-      <c r="C2" s="39">
+      <c r="C2" s="37">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -2629,7 +2627,7 @@
       <c r="B3" s="6">
         <v>1</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="37">
         <v>0.9</v>
       </c>
     </row>
@@ -2640,7 +2638,7 @@
       <c r="B4" s="6">
         <v>0</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="37">
         <v>1.5</v>
       </c>
     </row>
@@ -2651,7 +2649,7 @@
       <c r="B5" s="6">
         <v>1</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="37">
         <v>1.3</v>
       </c>
     </row>
@@ -2662,7 +2660,7 @@
       <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="37">
         <v>0.2</v>
       </c>
     </row>
@@ -2673,7 +2671,7 @@
       <c r="B7" s="6">
         <v>0</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="37">
         <v>1.7</v>
       </c>
     </row>
@@ -2684,7 +2682,7 @@
       <c r="B8" s="6">
         <v>1</v>
       </c>
-      <c r="C8" s="39">
+      <c r="C8" s="37">
         <v>1.4</v>
       </c>
     </row>
@@ -2695,7 +2693,7 @@
       <c r="B9" s="6">
         <v>2</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="37">
         <v>0.7</v>
       </c>
     </row>
@@ -2706,7 +2704,7 @@
       <c r="B10" s="6">
         <v>3</v>
       </c>
-      <c r="C10" s="39">
+      <c r="C10" s="37">
         <v>0.2</v>
       </c>
     </row>
@@ -2727,10 +2725,10 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2830,9 +2828,9 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2935,65 +2933,65 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="41" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" style="41" customWidth="1"/>
-    <col min="3" max="16384" width="14" style="41"/>
+    <col min="1" max="1" width="5.7109375" style="39" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="39" customWidth="1"/>
+    <col min="3" max="16384" width="14" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="38" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.4">
-      <c r="A2" s="42" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="43">
+      <c r="B2" s="41">
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14.4">
-      <c r="A3" s="44">
+    <row r="3" spans="1:2">
+      <c r="A3" s="42">
         <v>44123</v>
       </c>
-      <c r="B3" s="43">
+      <c r="B3" s="41">
         <v>1.17E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14.4">
-      <c r="A4" s="42" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="43">
+      <c r="B4" s="41">
         <v>6.8099999999999994E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="14.4">
-      <c r="A5" s="42" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="43">
+      <c r="B5" s="41">
         <v>0.27179999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="14.4">
-      <c r="A6" s="42" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="43">
+      <c r="B6" s="41">
         <v>0.32050000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="14.4">
-      <c r="A7" s="42">
+    <row r="7" spans="1:2">
+      <c r="A7" s="40">
         <f>70</f>
         <v>70</v>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="41">
         <v>0.3261</v>
       </c>
     </row>
@@ -3017,284 +3015,284 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="41" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" style="41" customWidth="1"/>
-    <col min="4" max="16384" width="14" style="41"/>
+    <col min="1" max="1" width="28.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="39" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="39" customWidth="1"/>
+    <col min="4" max="16384" width="14" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="47" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="48" t="s">
         <v>210</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="47" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="46" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="46" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="46" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="46" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="46" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="46" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="46" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="46" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="46" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="46" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="46" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="46" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="C14" s="46" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="C19" s="51" t="s">
+      <c r="C19" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="C20" s="51" t="s">
+      <c r="C20" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="C21" s="51" t="s">
+      <c r="C21" s="46" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="C22" s="51" t="s">
+      <c r="C22" s="46" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="46" t="s">
         <v>212</v>
       </c>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="C23" s="46" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="51" t="s">
+      <c r="C24" s="46" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.4">
+    <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="51" t="s">
+      <c r="B25" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="C25" s="51" t="s">
+      <c r="C25" s="46" t="s">
         <v>106</v>
       </c>
     </row>
@@ -3302,10 +3300,10 @@
       <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="51" t="s">
+      <c r="B26" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="51" t="s">
+      <c r="C26" s="46" t="s">
         <v>106</v>
       </c>
     </row>
@@ -3326,11 +3324,11 @@
       <selection activeCell="H2720" sqref="H2720"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -63302,574 +63300,574 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="14" style="41"/>
+    <col min="1" max="1" width="33.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="14" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="43" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="42">
+      <c r="B2" s="40">
         <v>61659</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="44" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="42">
+      <c r="B3" s="40">
         <v>5273</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="44" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="42">
+      <c r="B4" s="40">
         <v>3866</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="40" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="42">
+      <c r="B5" s="40">
         <v>3194</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="40" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="42">
+      <c r="B6" s="40">
         <v>5640</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="40" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="B7" s="42">
+      <c r="B7" s="40">
         <v>1248</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="40" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="B8" s="42">
+      <c r="B8" s="40">
         <v>3945</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="40" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="B9" s="42">
+      <c r="B9" s="40">
         <v>1039</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="40" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="B10" s="42">
+      <c r="B10" s="40">
         <v>75729</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="40" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="B11" s="42">
+      <c r="B11" s="40">
         <v>1188</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="40" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="B12" s="42">
+      <c r="B12" s="40">
         <v>4058</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="40" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="42">
+      <c r="B13" s="40">
         <v>1032</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="40" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="B14" s="42">
+      <c r="B14" s="40">
         <v>924</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="40" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="B15" s="42">
+      <c r="B15" s="40">
         <v>396</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="40" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="42">
+      <c r="B16" s="40">
         <v>374</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="40" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="B17" s="42">
+      <c r="B17" s="40">
         <v>100</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="40" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="B18" s="42">
+      <c r="B18" s="40">
         <v>436</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="40" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="42">
+      <c r="B19" s="40">
         <v>420</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="40" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="B20" s="42">
+      <c r="B20" s="40">
         <v>4218</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="40" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="B21" s="42">
+      <c r="B21" s="40">
         <v>23</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="40" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="42">
+      <c r="B22" s="40">
         <v>8345</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="40" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="42">
+      <c r="B23" s="40">
         <v>1111</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="40" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="B24" s="42">
+      <c r="B24" s="40">
         <v>967</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="40" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="42">
+      <c r="B25" s="40">
         <v>239</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="40" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="B26" s="42">
+      <c r="B26" s="40">
         <v>721</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="40" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="B27" s="42">
+      <c r="B27" s="40">
         <v>112</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="40" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="42">
+      <c r="B28" s="40">
         <v>613</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="40" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="B29" s="42">
+      <c r="B29" s="40">
         <v>243</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="40" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="B30" s="42">
+      <c r="B30" s="40">
         <v>2106</v>
       </c>
-      <c r="C30" s="42" t="s">
+      <c r="C30" s="40" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="B31" s="42">
+      <c r="B31" s="40">
         <v>142</v>
       </c>
-      <c r="C31" s="42" t="s">
+      <c r="C31" s="40" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="42" t="s">
+      <c r="A32" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="B32" s="42">
+      <c r="B32" s="40">
         <v>10740</v>
       </c>
-      <c r="C32" s="42" t="s">
+      <c r="C32" s="40" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="42" t="s">
+      <c r="A33" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="42">
+      <c r="B33" s="40">
         <v>2052</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="40" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="B34" s="42">
+      <c r="B34" s="40">
         <v>1783</v>
       </c>
-      <c r="C34" s="42" t="s">
+      <c r="C34" s="40" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="42" t="s">
+      <c r="A35" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="B35" s="42">
+      <c r="B35" s="40">
         <v>1357</v>
       </c>
-      <c r="C35" s="42" t="s">
+      <c r="C35" s="40" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="B36" s="42">
+      <c r="B36" s="40">
         <v>1134</v>
       </c>
-      <c r="C36" s="42" t="s">
+      <c r="C36" s="40" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="42" t="s">
+      <c r="A37" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="B37" s="42">
+      <c r="B37" s="40">
         <v>281</v>
       </c>
-      <c r="C37" s="42" t="s">
+      <c r="C37" s="40" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="42" t="s">
+      <c r="A38" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="B38" s="42">
+      <c r="B38" s="40">
         <v>1073</v>
       </c>
-      <c r="C38" s="42" t="s">
+      <c r="C38" s="40" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="42" t="s">
+      <c r="A39" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="42">
+      <c r="B39" s="40">
         <v>630</v>
       </c>
-      <c r="C39" s="42" t="s">
+      <c r="C39" s="40" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="42" t="s">
+      <c r="A40" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="B40" s="42">
+      <c r="B40" s="40">
         <v>2246</v>
       </c>
-      <c r="C40" s="42" t="s">
+      <c r="C40" s="40" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="42" t="s">
+      <c r="A41" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="B41" s="42">
+      <c r="B41" s="40">
         <v>271</v>
       </c>
-      <c r="C41" s="42" t="s">
+      <c r="C41" s="40" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="42" t="s">
+      <c r="A42" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="B42" s="42">
+      <c r="B42" s="40">
         <v>4512</v>
       </c>
-      <c r="C42" s="42" t="s">
+      <c r="C42" s="40" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="42" t="s">
+      <c r="A43" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="B43" s="42">
+      <c r="B43" s="40">
         <v>877</v>
       </c>
-      <c r="C43" s="42" t="s">
+      <c r="C43" s="40" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="42" t="s">
+      <c r="A44" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="B44" s="42">
+      <c r="B44" s="40">
         <v>961</v>
       </c>
-      <c r="C44" s="42" t="s">
+      <c r="C44" s="40" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="42" t="s">
+      <c r="A45" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="B45" s="42">
+      <c r="B45" s="40">
         <v>748</v>
       </c>
-      <c r="C45" s="42" t="s">
+      <c r="C45" s="40" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="42" t="s">
+      <c r="A46" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="B46" s="42">
+      <c r="B46" s="40">
         <v>424</v>
       </c>
-      <c r="C46" s="42" t="s">
+      <c r="C46" s="40" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="42" t="s">
+      <c r="A47" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="B47" s="42">
+      <c r="B47" s="40">
         <v>82</v>
       </c>
-      <c r="C47" s="42" t="s">
+      <c r="C47" s="40" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="42" t="s">
+      <c r="A48" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="B48" s="42">
+      <c r="B48" s="40">
         <v>435</v>
       </c>
-      <c r="C48" s="42" t="s">
+      <c r="C48" s="40" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="42" t="s">
+      <c r="A49" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="B49" s="42">
+      <c r="B49" s="40">
         <v>221</v>
       </c>
-      <c r="C49" s="42" t="s">
+      <c r="C49" s="40" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="42" t="s">
+      <c r="A50" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="B50" s="42">
+      <c r="B50" s="40">
         <v>1485</v>
       </c>
-      <c r="C50" s="42" t="s">
+      <c r="C50" s="40" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="42" t="s">
+      <c r="A51" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="B51" s="42">
+      <c r="B51" s="40">
         <v>237</v>
       </c>
-      <c r="C51" s="42" t="s">
+      <c r="C51" s="40" t="s">
         <v>121</v>
       </c>
     </row>
@@ -63890,7 +63888,7 @@
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" t="s">
@@ -65992,736 +65990,736 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" style="41" customWidth="1"/>
-    <col min="2" max="2" width="31" style="41" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" style="41" customWidth="1"/>
-    <col min="4" max="4" width="14" style="41"/>
-    <col min="5" max="5" width="26.88671875" style="41" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="41" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="41" customWidth="1"/>
-    <col min="8" max="16384" width="14" style="41"/>
+    <col min="1" max="1" width="37.28515625" style="39" customWidth="1"/>
+    <col min="2" max="2" width="31" style="39" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" style="39" customWidth="1"/>
+    <col min="4" max="4" width="14" style="39"/>
+    <col min="5" max="5" width="26.85546875" style="39" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="39" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="39" customWidth="1"/>
+    <col min="8" max="16384" width="14" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="51"/>
+      <c r="C2" s="46"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="51">
+      <c r="C3" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="46" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="46" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="46" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="46" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="46" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="46" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="46" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="46" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="46" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="46" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="C14" s="46" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="46" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="46" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="46" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="46" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="C19" s="51" t="s">
+      <c r="C19" s="46" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="51" t="s">
+      <c r="C20" s="46" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="51" t="s">
+      <c r="C21" s="46" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="C22" s="51" t="s">
+      <c r="C22" s="46" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="C23" s="46" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="C24" s="51" t="s">
+      <c r="C24" s="46" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="B25" s="51" t="s">
+      <c r="B25" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="C25" s="51" t="s">
+      <c r="C25" s="46" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="51" t="s">
+      <c r="A26" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="B26" s="51" t="s">
+      <c r="B26" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="C26" s="51" t="s">
+      <c r="C26" s="46" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="51" t="s">
+      <c r="A27" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="C27" s="51" t="s">
+      <c r="C27" s="46" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="B28" s="51" t="s">
+      <c r="B28" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="C28" s="51" t="s">
+      <c r="C28" s="46" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="C29" s="51" t="s">
+      <c r="C29" s="46" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="B30" s="51" t="s">
+      <c r="B30" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="C30" s="51" t="s">
+      <c r="C30" s="46" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="B31" s="51" t="s">
+      <c r="B31" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="C31" s="51" t="s">
+      <c r="C31" s="46" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="B32" s="51" t="s">
+      <c r="B32" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="C32" s="51" t="s">
+      <c r="C32" s="46" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="B33" s="51" t="s">
+      <c r="B33" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="C33" s="51" t="s">
+      <c r="C33" s="46" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="B34" s="51" t="s">
+      <c r="B34" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="C34" s="51" t="s">
+      <c r="C34" s="46" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="51" t="s">
+      <c r="A35" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="51" t="s">
+      <c r="B35" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="C35" s="51" t="s">
+      <c r="C35" s="46" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="51" t="s">
+      <c r="A36" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="C36" s="51" t="s">
+      <c r="C36" s="46" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="51" t="s">
+      <c r="A37" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="B37" s="51" t="s">
+      <c r="B37" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="C37" s="51" t="s">
+      <c r="C37" s="46" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="51" t="s">
+      <c r="A38" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="B38" s="51" t="s">
+      <c r="B38" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="C38" s="51" t="s">
+      <c r="C38" s="46" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="51" t="s">
+      <c r="A39" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="B39" s="51" t="s">
+      <c r="B39" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="51" t="s">
+      <c r="C39" s="46" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="51" t="s">
+      <c r="A40" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="B40" s="51" t="s">
+      <c r="B40" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="C40" s="51" t="s">
+      <c r="C40" s="46" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="51" t="s">
+      <c r="A41" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="B41" s="51" t="s">
+      <c r="B41" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="C41" s="51" t="s">
+      <c r="C41" s="46" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="51" t="s">
+      <c r="A42" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="B42" s="51" t="s">
+      <c r="B42" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="C42" s="51" t="s">
+      <c r="C42" s="46" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="51" t="s">
+      <c r="A43" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="51" t="s">
+      <c r="B43" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="C43" s="51" t="s">
+      <c r="C43" s="46" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="51" t="s">
+      <c r="A44" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="B44" s="51" t="s">
+      <c r="B44" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="C44" s="51" t="s">
+      <c r="C44" s="46" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="51" t="s">
+      <c r="A45" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="B45" s="51" t="s">
+      <c r="B45" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="C45" s="51" t="s">
+      <c r="C45" s="46" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="51" t="s">
+      <c r="A46" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="B46" s="51" t="s">
+      <c r="B46" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="C46" s="51" t="s">
+      <c r="C46" s="46" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="51" t="s">
+      <c r="A47" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="B47" s="51" t="s">
+      <c r="B47" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="C47" s="51" t="s">
+      <c r="C47" s="46" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="51" t="s">
+      <c r="A48" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="B48" s="51" t="s">
+      <c r="B48" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="C48" s="51" t="s">
+      <c r="C48" s="46" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="51" t="s">
+      <c r="A49" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="B49" s="51" t="s">
+      <c r="B49" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="C49" s="51" t="s">
+      <c r="C49" s="46" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="51" t="s">
+      <c r="A50" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="B50" s="51" t="s">
+      <c r="B50" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="C50" s="51" t="s">
+      <c r="C50" s="46" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="51" t="s">
+      <c r="A51" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="51" t="s">
+      <c r="B51" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="C51" s="51" t="s">
+      <c r="C51" s="46" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="51" t="s">
+      <c r="A52" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="B52" s="51" t="s">
+      <c r="B52" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="C52" s="51" t="s">
+      <c r="C52" s="46" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="51" t="s">
+      <c r="A53" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="B53" s="51" t="s">
+      <c r="B53" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="C53" s="51" t="s">
+      <c r="C53" s="46" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="51" t="s">
+      <c r="A54" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="B54" s="51" t="s">
+      <c r="B54" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="C54" s="51" t="s">
+      <c r="C54" s="46" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="51" t="s">
+      <c r="A55" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="B55" s="51" t="s">
+      <c r="B55" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="C55" s="51" t="s">
+      <c r="C55" s="46" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="51" t="s">
+      <c r="A56" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="B56" s="51" t="s">
+      <c r="B56" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="C56" s="51" t="s">
+      <c r="C56" s="46" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="51" t="s">
+      <c r="A57" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="B57" s="51" t="s">
+      <c r="B57" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="C57" s="51" t="s">
+      <c r="C57" s="46" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="51" t="s">
+      <c r="A58" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="B58" s="51" t="s">
+      <c r="B58" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="C58" s="51" t="s">
+      <c r="C58" s="46" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="51" t="s">
+      <c r="A59" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B59" s="51" t="s">
+      <c r="B59" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="C59" s="51" t="s">
+      <c r="C59" s="46" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="51" t="s">
+      <c r="A60" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="B60" s="51" t="s">
+      <c r="B60" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="C60" s="51" t="s">
+      <c r="C60" s="46" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="51" t="s">
+      <c r="A61" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="B61" s="51" t="s">
+      <c r="B61" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="C61" s="51" t="s">
+      <c r="C61" s="46" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="51" t="s">
+      <c r="A62" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="B62" s="51" t="s">
+      <c r="B62" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="C62" s="51" t="s">
+      <c r="C62" s="46" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="51" t="s">
+      <c r="A63" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="B63" s="51" t="s">
+      <c r="B63" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="C63" s="51" t="s">
+      <c r="C63" s="46" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="51" t="s">
+      <c r="A64" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="B64" s="51" t="s">
+      <c r="B64" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="C64" s="51" t="s">
+      <c r="C64" s="46" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="51" t="s">
+      <c r="A65" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="B65" s="51" t="s">
+      <c r="B65" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="C65" s="51" t="s">
+      <c r="C65" s="46" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="51" t="s">
+      <c r="A66" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="B66" s="51" t="s">
+      <c r="B66" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="C66" s="51" t="s">
+      <c r="C66" s="46" t="s">
         <v>192</v>
       </c>
     </row>
@@ -66748,71 +66746,71 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.77734375" style="41" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="41" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" style="41" customWidth="1"/>
-    <col min="4" max="16384" width="14" style="41"/>
+    <col min="1" max="1" width="27.7109375" style="39" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="39" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="39" customWidth="1"/>
+    <col min="4" max="16384" width="14" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="46" t="s">
         <v>194</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="46" t="s">
         <v>195</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="46" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="46" t="s">
         <v>197</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="46" t="s">
         <v>198</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="46" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="46" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="46" t="s">
         <v>204</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="46" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="46" t="s">
         <v>206</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="46" t="s">
         <v>207</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="46" t="s">
         <v>208</v>
       </c>
     </row>
@@ -66836,17 +66834,17 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="76" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="198.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="30"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="198.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -66866,7 +66864,7 @@
       <c r="G1"/>
       <c r="H1"/>
     </row>
-    <row r="2" spans="1:8" ht="140.4">
+    <row r="2" spans="1:8" ht="141.75">
       <c r="A2" s="11" t="s">
         <v>44</v>
       </c>
@@ -66886,7 +66884,7 @@
       <c r="G2" s="26"/>
       <c r="H2" s="26"/>
     </row>
-    <row r="3" spans="1:8" ht="15.6">
+    <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="16" t="s">
         <v>47</v>
       </c>
@@ -66904,7 +66902,7 @@
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
     </row>
-    <row r="4" spans="1:8" ht="15.6">
+    <row r="4" spans="1:8" ht="15.75">
       <c r="A4" s="21" t="s">
         <v>49</v>
       </c>
@@ -66924,7 +66922,7 @@
       <c r="G4" s="28"/>
       <c r="H4" s="28"/>
     </row>
-    <row r="5" spans="1:8" ht="15.6">
+    <row r="5" spans="1:8" ht="15.75">
       <c r="A5" s="16" t="s">
         <v>51</v>
       </c>
@@ -66942,7 +66940,7 @@
       <c r="G5" s="27"/>
       <c r="H5" s="27"/>
     </row>
-    <row r="6" spans="1:8" ht="15.6">
+    <row r="6" spans="1:8" ht="15.75">
       <c r="A6" s="8" t="s">
         <v>54</v>
       </c>
@@ -66962,7 +66960,7 @@
       <c r="G6" s="27"/>
       <c r="H6" s="27"/>
     </row>
-    <row r="7" spans="1:8" ht="15.6">
+    <row r="7" spans="1:8" ht="15.75">
       <c r="A7" s="8" t="s">
         <v>56</v>
       </c>
@@ -66982,7 +66980,7 @@
       <c r="G7" s="29"/>
       <c r="H7" s="29"/>
     </row>
-    <row r="8" spans="1:8" ht="46.8">
+    <row r="8" spans="1:8" ht="47.25">
       <c r="A8" s="8" t="s">
         <v>58</v>
       </c>
@@ -67002,7 +67000,7 @@
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
     </row>
-    <row r="9" spans="1:8" ht="15.6">
+    <row r="9" spans="1:8" ht="15.75">
       <c r="A9" s="8" t="s">
         <v>60</v>
       </c>
@@ -67022,7 +67020,7 @@
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:8" ht="15.6">
+    <row r="10" spans="1:8" ht="15.75">
       <c r="A10" s="8" t="s">
         <v>64</v>
       </c>
@@ -67042,7 +67040,7 @@
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="1:8" ht="15.6">
+    <row r="11" spans="1:8" ht="15.75">
       <c r="A11" s="11" t="s">
         <v>67</v>
       </c>
@@ -67062,7 +67060,7 @@
       <c r="G11" s="27"/>
       <c r="H11" s="27"/>
     </row>
-    <row r="12" spans="1:8" ht="15.6">
+    <row r="12" spans="1:8" ht="15.75">
       <c r="A12" s="8" t="s">
         <v>71</v>
       </c>
@@ -67082,7 +67080,7 @@
       <c r="G12" s="27"/>
       <c r="H12" s="27"/>
     </row>
-    <row r="13" spans="1:8" ht="15.6">
+    <row r="13" spans="1:8" ht="15.75">
       <c r="A13" s="8" t="s">
         <v>74</v>
       </c>
@@ -67102,7 +67100,7 @@
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
     </row>
-    <row r="14" spans="1:8" ht="15.6">
+    <row r="14" spans="1:8" ht="15.75">
       <c r="A14" s="16" t="s">
         <v>76</v>
       </c>
@@ -67112,7 +67110,7 @@
       <c r="C14" s="18">
         <v>16</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="52" t="s">
         <v>88</v>
       </c>
       <c r="E14" s="16" t="s">
@@ -67122,7 +67120,7 @@
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
     </row>
-    <row r="15" spans="1:8" ht="15.6">
+    <row r="15" spans="1:8" ht="15.75">
       <c r="A15" s="16" t="s">
         <v>78</v>
       </c>
@@ -67132,7 +67130,7 @@
       <c r="C15" s="18">
         <v>8</v>
       </c>
-      <c r="D15" s="34"/>
+      <c r="D15" s="53"/>
       <c r="E15" s="16" t="s">
         <v>46</v>
       </c>
@@ -67164,120 +67162,120 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="36">
+      <c r="A2" s="34">
         <v>0</v>
       </c>
-      <c r="B2" s="37">
+      <c r="B2" s="35">
         <v>0</v>
       </c>
-      <c r="C2" s="38">
+      <c r="C2" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="36">
+      <c r="A3" s="34">
         <v>10</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="35">
         <v>1E-4</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="36">
         <v>2E-3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="36">
+      <c r="A4" s="34">
         <v>20</v>
       </c>
-      <c r="B4" s="37">
+      <c r="B4" s="35">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="36">
         <v>2E-3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="36">
+      <c r="A5" s="34">
         <v>30</v>
       </c>
-      <c r="B5" s="37">
+      <c r="B5" s="35">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="36">
         <v>2E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="36">
+      <c r="A6" s="34">
         <v>40</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B6" s="35">
         <v>1.5E-3</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="36">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="36">
+      <c r="A7" s="34">
         <v>50</v>
       </c>
-      <c r="B7" s="37">
+      <c r="B7" s="35">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="36">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="36">
+      <c r="A8" s="34">
         <v>60</v>
       </c>
-      <c r="B8" s="37">
+      <c r="B8" s="35">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="36">
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="36">
+      <c r="A9" s="34">
         <v>70</v>
       </c>
-      <c r="B9" s="37">
+      <c r="B9" s="35">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="36">
         <v>0.08</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="36">
+      <c r="A10" s="34">
         <v>80</v>
       </c>
-      <c r="B10" s="37">
+      <c r="B10" s="35">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="36">
         <v>0.14799999999999999</v>
       </c>
     </row>

</xml_diff>